<commit_message>
Added excel code and changed around writing
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="630" yWindow="600" windowWidth="27495" windowHeight="13740" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -26,7 +25,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
       <b val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,10 +47,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -62,7 +72,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -427,11 +437,17 @@
   </sheetPr>
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="60" customWidth="1" min="1" max="1"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="3" max="3"/>
+    <col width="30" customWidth="1" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -454,11 +470,7 @@
           <t>Exit rate</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Unnamed: 4</t>
-        </is>
-      </c>
+      <c r="E1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -481,7 +493,6 @@
           <t>89%</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -504,7 +515,6 @@
           <t>91%</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -527,7 +537,6 @@
           <t>100%</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -550,7 +559,6 @@
           <t>63%</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -573,7 +581,6 @@
           <t>60%</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -596,7 +603,6 @@
           <t>36%</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -619,7 +625,6 @@
           <t>60%</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -642,7 +647,6 @@
           <t>73%</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -665,7 +669,6 @@
           <t>94%</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -688,7 +691,6 @@
           <t>82%</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -711,7 +713,6 @@
           <t>60%</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -734,7 +735,6 @@
           <t>67%</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -757,7 +757,6 @@
           <t>48%</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -780,7 +779,6 @@
           <t>36%</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -803,7 +801,6 @@
           <t>91%</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -826,7 +823,6 @@
           <t>28%</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -849,7 +845,6 @@
           <t>77%</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -872,7 +867,6 @@
           <t>43%</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -895,7 +889,6 @@
           <t>67%</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -918,7 +911,6 @@
           <t>50%</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -941,7 +933,6 @@
           <t>85%</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -964,7 +955,6 @@
           <t>56%</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -987,7 +977,6 @@
           <t>44%</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1010,7 +999,6 @@
           <t>76%</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1033,7 +1021,6 @@
           <t>40%</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1051,8 +1038,6 @@
           <t>Clicks</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1070,8 +1055,6 @@
           <t>790</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1089,8 +1072,6 @@
           <t>688</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1108,8 +1089,6 @@
           <t>355</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1127,8 +1106,6 @@
           <t>134</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1146,8 +1123,6 @@
           <t>31</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1165,8 +1140,6 @@
           <t>32</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1184,8 +1157,6 @@
           <t>23</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1203,8 +1174,6 @@
           <t>21</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1222,8 +1191,6 @@
           <t>18</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1241,8 +1208,6 @@
           <t>10</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1260,8 +1225,6 @@
           <t>12</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1279,8 +1242,6 @@
           <t>11</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1298,8 +1259,6 @@
           <t>10</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1317,8 +1276,6 @@
           <t>8</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1336,8 +1293,6 @@
           <t>5</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1355,8 +1310,6 @@
           <t>5</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1374,8 +1327,6 @@
           <t>5</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1393,8 +1344,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1412,8 +1361,6 @@
           <t>3</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1431,8 +1378,6 @@
           <t>3</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr"/>
-      <c r="E47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1450,8 +1395,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr"/>
-      <c r="E48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1469,8 +1412,6 @@
           <t>3</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1488,8 +1429,6 @@
           <t>3</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1507,8 +1446,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr"/>
-      <c r="E51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1526,8 +1463,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr"/>
-      <c r="E52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1540,9 +1475,6 @@
           <t>Visits</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr"/>
-      <c r="D53" t="inlineStr"/>
-      <c r="E53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1555,9 +1487,6 @@
           <t>228</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr"/>
-      <c r="E54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1570,9 +1499,6 @@
           <t>191</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr"/>
-      <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1585,9 +1511,6 @@
           <t>66</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr"/>
-      <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1600,9 +1523,6 @@
           <t>63</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr"/>
-      <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1615,9 +1535,6 @@
           <t>41</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr"/>
-      <c r="D58" t="inlineStr"/>
-      <c r="E58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1630,9 +1547,6 @@
           <t>19</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr"/>
-      <c r="D59" t="inlineStr"/>
-      <c r="E59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1645,9 +1559,6 @@
           <t>12</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr"/>
-      <c r="D60" t="inlineStr"/>
-      <c r="E60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1660,9 +1571,6 @@
           <t>10</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr"/>
-      <c r="E61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1675,9 +1583,6 @@
           <t>7</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr"/>
-      <c r="D62" t="inlineStr"/>
-      <c r="E62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1690,9 +1595,6 @@
           <t>6</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr"/>
-      <c r="D63" t="inlineStr"/>
-      <c r="E63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1705,9 +1607,6 @@
           <t>6</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr"/>
-      <c r="D64" t="inlineStr"/>
-      <c r="E64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1720,9 +1619,6 @@
           <t>6</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr"/>
-      <c r="D65" t="inlineStr"/>
-      <c r="E65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1735,9 +1631,6 @@
           <t>5</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr"/>
-      <c r="D66" t="inlineStr"/>
-      <c r="E66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1750,9 +1643,6 @@
           <t>5</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr"/>
-      <c r="D67" t="inlineStr"/>
-      <c r="E67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1765,9 +1655,6 @@
           <t>4</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr"/>
-      <c r="D68" t="inlineStr"/>
-      <c r="E68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1780,9 +1667,6 @@
           <t>3</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr"/>
-      <c r="D69" t="inlineStr"/>
-      <c r="E69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1795,9 +1679,6 @@
           <t>3</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr"/>
-      <c r="D70" t="inlineStr"/>
-      <c r="E70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1810,9 +1691,6 @@
           <t>3</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr"/>
-      <c r="E71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1825,9 +1703,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr"/>
-      <c r="E72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1840,9 +1715,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr"/>
-      <c r="D73" t="inlineStr"/>
-      <c r="E73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1855,9 +1727,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr"/>
-      <c r="D74" t="inlineStr"/>
-      <c r="E74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1870,9 +1739,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr"/>
-      <c r="D75" t="inlineStr"/>
-      <c r="E75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1885,9 +1751,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr"/>
-      <c r="D76" t="inlineStr"/>
-      <c r="E76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1900,9 +1763,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="C77" t="inlineStr"/>
-      <c r="D77" t="inlineStr"/>
-      <c r="E77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1915,9 +1775,6 @@
           <t>2</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr"/>
-      <c r="D78" t="inlineStr"/>
-      <c r="E78" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>